<commit_message>
New Code Is Added 01/06/2025
</commit_message>
<xml_diff>
--- a/ExcelFiles/LOGIN.xlsx
+++ b/ExcelFiles/LOGIN.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANKUSH\NEW_HORIZON\ExcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Ahmedabad\ANKUSH_FRAMEWORK\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6717E388-B489-4812-8136-6A8609442FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142D1EFA-8795-475F-B55E-510FF3160643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="LOGIN" sheetId="2" r:id="rId1"/>
+    <sheet name="JDBC" sheetId="3" r:id="rId1"/>
+    <sheet name="LOGIN" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>su</t>
   </si>
@@ -118,12 +119,51 @@
       <t>ELI-PRD</t>
     </r>
   </si>
+  <si>
+    <t>SQLSERVER</t>
+  </si>
+  <si>
+    <t>DATABASE</t>
+  </si>
+  <si>
+    <t>ADMIN_DATABASE</t>
+  </si>
+  <si>
+    <t>USER</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>encrypt</t>
+  </si>
+  <si>
+    <t>trustServerCertificate</t>
+  </si>
+  <si>
+    <t>loginTimeout</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>QADEMO</t>
+  </si>
+  <si>
+    <t>localhost:1433</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +195,14 @@
       <color rgb="FF2A00FF"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -204,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -212,6 +260,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,20 +543,87 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D9D3596-9849-4B9C-B628-7C8B473D0484}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB6998C4-7D97-469A-A3EF-FF8EB1B70410}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="103.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D9D3596-9849-4B9C-B628-7C8B473D0484}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="103.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -513,7 +631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -521,7 +639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -529,7 +647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -537,7 +655,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -545,7 +663,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>